<commit_message>
Calculate percentage after after march
</commit_message>
<xml_diff>
--- a/Output/Excel/df_month.xlsx
+++ b/Output/Excel/df_month.xlsx
@@ -1174,7 +1174,7 @@
         <v>2002</v>
       </c>
       <c r="BC4" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD4" t="inlineStr"/>
       <c r="BE4" t="inlineStr"/>
@@ -1327,7 +1327,7 @@
         <v>2002</v>
       </c>
       <c r="BC5" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD5" t="inlineStr"/>
       <c r="BE5" t="inlineStr"/>
@@ -1480,7 +1480,7 @@
         <v>2002</v>
       </c>
       <c r="BC6" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD6" t="inlineStr"/>
       <c r="BE6" t="inlineStr"/>
@@ -1633,7 +1633,7 @@
         <v>2002</v>
       </c>
       <c r="BC7" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD7" t="inlineStr"/>
       <c r="BE7" t="inlineStr"/>
@@ -1786,7 +1786,7 @@
         <v>2002</v>
       </c>
       <c r="BC8" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD8" t="inlineStr"/>
       <c r="BE8" t="inlineStr"/>
@@ -1939,7 +1939,7 @@
         <v>2002</v>
       </c>
       <c r="BC9" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD9" t="inlineStr"/>
       <c r="BE9" t="inlineStr"/>
@@ -2092,7 +2092,7 @@
         <v>2002</v>
       </c>
       <c r="BC10" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD10" t="inlineStr"/>
       <c r="BE10" t="inlineStr"/>
@@ -2245,7 +2245,7 @@
         <v>2003</v>
       </c>
       <c r="BC11" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD11" t="inlineStr"/>
       <c r="BE11" t="inlineStr"/>
@@ -2398,7 +2398,7 @@
         <v>2003</v>
       </c>
       <c r="BC12" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD12" t="inlineStr"/>
       <c r="BE12" t="inlineStr"/>
@@ -2551,7 +2551,7 @@
         <v>2003</v>
       </c>
       <c r="BC13" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD13" t="inlineStr"/>
       <c r="BE13" t="inlineStr"/>
@@ -2704,7 +2704,7 @@
         <v>2003</v>
       </c>
       <c r="BC14" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD14" t="inlineStr"/>
       <c r="BE14" t="inlineStr"/>
@@ -2857,7 +2857,7 @@
         <v>2003</v>
       </c>
       <c r="BC15" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BD15" t="inlineStr"/>
       <c r="BE15" t="inlineStr"/>
@@ -3010,7 +3010,7 @@
         <v>2003</v>
       </c>
       <c r="BC16" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD16" t="inlineStr"/>
       <c r="BE16" t="inlineStr"/>
@@ -3163,7 +3163,7 @@
         <v>2003</v>
       </c>
       <c r="BC17" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD17" t="inlineStr"/>
       <c r="BE17" t="inlineStr"/>
@@ -3316,10 +3316,10 @@
         <v>2003</v>
       </c>
       <c r="BC18" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD18" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE18" t="inlineStr"/>
     </row>
@@ -3471,10 +3471,10 @@
         <v>2003</v>
       </c>
       <c r="BC19" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD19" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE19" t="inlineStr"/>
     </row>
@@ -3626,10 +3626,10 @@
         <v>2003</v>
       </c>
       <c r="BC20" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD20" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE20" t="inlineStr"/>
     </row>
@@ -3781,10 +3781,10 @@
         <v>2003</v>
       </c>
       <c r="BC21" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD21" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE21" t="inlineStr"/>
     </row>
@@ -3936,10 +3936,10 @@
         <v>2003</v>
       </c>
       <c r="BC22" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD22" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE22" t="inlineStr"/>
     </row>
@@ -4091,10 +4091,10 @@
         <v>2004</v>
       </c>
       <c r="BC23" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD23" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE23" t="inlineStr"/>
     </row>
@@ -4246,10 +4246,10 @@
         <v>2004</v>
       </c>
       <c r="BC24" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD24" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE24" t="inlineStr"/>
     </row>
@@ -4401,10 +4401,10 @@
         <v>2004</v>
       </c>
       <c r="BC25" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD25" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE25" t="inlineStr"/>
     </row>
@@ -4556,10 +4556,10 @@
         <v>2004</v>
       </c>
       <c r="BC26" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD26" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE26" t="inlineStr"/>
     </row>
@@ -4711,10 +4711,10 @@
         <v>2004</v>
       </c>
       <c r="BC27" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BD27" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE27" t="inlineStr"/>
     </row>
@@ -4866,10 +4866,10 @@
         <v>2004</v>
       </c>
       <c r="BC28" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD28" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE28" t="inlineStr"/>
     </row>
@@ -5021,10 +5021,10 @@
         <v>2004</v>
       </c>
       <c r="BC29" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD29" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
       <c r="BE29" t="inlineStr"/>
     </row>
@@ -5176,13 +5176,13 @@
         <v>2004</v>
       </c>
       <c r="BC30" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD30" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE30" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="31">
@@ -5333,13 +5333,13 @@
         <v>2004</v>
       </c>
       <c r="BC31" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD31" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE31" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="32">
@@ -5490,13 +5490,13 @@
         <v>2004</v>
       </c>
       <c r="BC32" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD32" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE32" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="33">
@@ -5647,13 +5647,13 @@
         <v>2004</v>
       </c>
       <c r="BC33" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD33" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE33" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="34">
@@ -5804,13 +5804,13 @@
         <v>2004</v>
       </c>
       <c r="BC34" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD34" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE34" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="35">
@@ -5961,13 +5961,13 @@
         <v>2005</v>
       </c>
       <c r="BC35" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD35" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE35" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="36">
@@ -6118,13 +6118,13 @@
         <v>2005</v>
       </c>
       <c r="BC36" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD36" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE36" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="37">
@@ -6275,13 +6275,13 @@
         <v>2005</v>
       </c>
       <c r="BC37" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD37" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE37" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="38">
@@ -6432,13 +6432,13 @@
         <v>2005</v>
       </c>
       <c r="BC38" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD38" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE38" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="39">
@@ -6589,13 +6589,13 @@
         <v>2005</v>
       </c>
       <c r="BC39" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BD39" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE39" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="40">
@@ -6746,13 +6746,13 @@
         <v>2005</v>
       </c>
       <c r="BC40" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD40" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE40" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="41">
@@ -6903,13 +6903,13 @@
         <v>2005</v>
       </c>
       <c r="BC41" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD41" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
       <c r="BE41" t="n">
-        <v>931.9</v>
+        <v>830.3</v>
       </c>
     </row>
     <row r="42">
@@ -7060,13 +7060,13 @@
         <v>2005</v>
       </c>
       <c r="BC42" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD42" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE42" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="43">
@@ -7217,13 +7217,13 @@
         <v>2005</v>
       </c>
       <c r="BC43" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD43" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE43" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="44">
@@ -7374,13 +7374,13 @@
         <v>2005</v>
       </c>
       <c r="BC44" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD44" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE44" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="45">
@@ -7531,13 +7531,13 @@
         <v>2005</v>
       </c>
       <c r="BC45" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD45" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE45" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="46">
@@ -7688,13 +7688,13 @@
         <v>2005</v>
       </c>
       <c r="BC46" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD46" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE46" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="47">
@@ -7845,13 +7845,13 @@
         <v>2006</v>
       </c>
       <c r="BC47" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD47" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE47" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="48">
@@ -8002,13 +8002,13 @@
         <v>2006</v>
       </c>
       <c r="BC48" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD48" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE48" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="49">
@@ -8159,13 +8159,13 @@
         <v>2006</v>
       </c>
       <c r="BC49" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD49" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE49" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="50">
@@ -8316,13 +8316,13 @@
         <v>2006</v>
       </c>
       <c r="BC50" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD50" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE50" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="51">
@@ -8473,13 +8473,13 @@
         <v>2006</v>
       </c>
       <c r="BC51" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BD51" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE51" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="52">
@@ -8630,13 +8630,13 @@
         <v>2006</v>
       </c>
       <c r="BC52" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD52" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE52" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="53">
@@ -8787,13 +8787,13 @@
         <v>2006</v>
       </c>
       <c r="BC53" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD53" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
       <c r="BE53" t="n">
-        <v>861.1</v>
+        <v>804.5</v>
       </c>
     </row>
     <row r="54">
@@ -8944,13 +8944,13 @@
         <v>2006</v>
       </c>
       <c r="BC54" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD54" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE54" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="55">
@@ -9101,13 +9101,13 @@
         <v>2006</v>
       </c>
       <c r="BC55" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD55" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE55" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="56">
@@ -9258,13 +9258,13 @@
         <v>2006</v>
       </c>
       <c r="BC56" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD56" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE56" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="57">
@@ -9415,13 +9415,13 @@
         <v>2006</v>
       </c>
       <c r="BC57" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD57" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE57" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="58">
@@ -9572,13 +9572,13 @@
         <v>2006</v>
       </c>
       <c r="BC58" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD58" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE58" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="59">
@@ -9729,13 +9729,13 @@
         <v>2007</v>
       </c>
       <c r="BC59" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD59" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE59" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="60">
@@ -9886,13 +9886,13 @@
         <v>2007</v>
       </c>
       <c r="BC60" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD60" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE60" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="61">
@@ -10043,13 +10043,13 @@
         <v>2007</v>
       </c>
       <c r="BC61" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD61" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE61" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="62">
@@ -10200,13 +10200,13 @@
         <v>2007</v>
       </c>
       <c r="BC62" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD62" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE62" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="63">
@@ -10357,13 +10357,13 @@
         <v>2007</v>
       </c>
       <c r="BC63" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BD63" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE63" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="64">
@@ -10514,13 +10514,13 @@
         <v>2007</v>
       </c>
       <c r="BC64" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD64" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE64" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="65">
@@ -10671,13 +10671,13 @@
         <v>2007</v>
       </c>
       <c r="BC65" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD65" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
       <c r="BE65" t="n">
-        <v>1416.6</v>
+        <v>1326.6</v>
       </c>
     </row>
     <row r="66">
@@ -10828,13 +10828,13 @@
         <v>2007</v>
       </c>
       <c r="BC66" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD66" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE66" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="67">
@@ -10985,13 +10985,13 @@
         <v>2007</v>
       </c>
       <c r="BC67" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD67" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE67" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="68">
@@ -11142,13 +11142,13 @@
         <v>2007</v>
       </c>
       <c r="BC68" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD68" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE68" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="69">
@@ -11299,13 +11299,13 @@
         <v>2007</v>
       </c>
       <c r="BC69" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD69" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE69" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="70">
@@ -11456,13 +11456,13 @@
         <v>2007</v>
       </c>
       <c r="BC70" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD70" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE70" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="71">
@@ -11613,13 +11613,13 @@
         <v>2008</v>
       </c>
       <c r="BC71" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD71" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE71" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="72">
@@ -11770,13 +11770,13 @@
         <v>2008</v>
       </c>
       <c r="BC72" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD72" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE72" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="73">
@@ -11927,13 +11927,13 @@
         <v>2008</v>
       </c>
       <c r="BC73" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD73" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE73" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="74">
@@ -12084,13 +12084,13 @@
         <v>2008</v>
       </c>
       <c r="BC74" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD74" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE74" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="75">
@@ -12241,13 +12241,13 @@
         <v>2008</v>
       </c>
       <c r="BC75" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BD75" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE75" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="76">
@@ -12398,13 +12398,13 @@
         <v>2008</v>
       </c>
       <c r="BC76" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD76" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE76" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="77">
@@ -12555,13 +12555,13 @@
         <v>2008</v>
       </c>
       <c r="BC77" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD77" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
       <c r="BE77" t="n">
-        <v>989.8000000000001</v>
+        <v>956.5</v>
       </c>
     </row>
     <row r="78">
@@ -12712,13 +12712,13 @@
         <v>2008</v>
       </c>
       <c r="BC78" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD78" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE78" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="79">
@@ -12869,13 +12869,13 @@
         <v>2008</v>
       </c>
       <c r="BC79" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD79" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE79" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="80">
@@ -13026,13 +13026,13 @@
         <v>2008</v>
       </c>
       <c r="BC80" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD80" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE80" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="81">
@@ -13183,13 +13183,13 @@
         <v>2008</v>
       </c>
       <c r="BC81" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD81" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE81" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="82">
@@ -13340,13 +13340,13 @@
         <v>2008</v>
       </c>
       <c r="BC82" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD82" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE82" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="83">
@@ -13497,13 +13497,13 @@
         <v>2009</v>
       </c>
       <c r="BC83" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD83" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE83" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="84">
@@ -13654,13 +13654,13 @@
         <v>2009</v>
       </c>
       <c r="BC84" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD84" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE84" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="85">
@@ -13811,13 +13811,13 @@
         <v>2009</v>
       </c>
       <c r="BC85" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD85" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE85" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="86">
@@ -13968,13 +13968,13 @@
         <v>2009</v>
       </c>
       <c r="BC86" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD86" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE86" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="87">
@@ -14125,13 +14125,13 @@
         <v>2009</v>
       </c>
       <c r="BC87" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BD87" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE87" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="88">
@@ -14282,13 +14282,13 @@
         <v>2009</v>
       </c>
       <c r="BC88" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD88" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE88" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="89">
@@ -14439,13 +14439,13 @@
         <v>2009</v>
       </c>
       <c r="BC89" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD89" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
       <c r="BE89" t="n">
-        <v>826.9</v>
+        <v>771.5</v>
       </c>
     </row>
     <row r="90">
@@ -14596,13 +14596,13 @@
         <v>2009</v>
       </c>
       <c r="BC90" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD90" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE90" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="91">
@@ -14753,13 +14753,13 @@
         <v>2009</v>
       </c>
       <c r="BC91" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD91" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE91" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="92">
@@ -14910,13 +14910,13 @@
         <v>2009</v>
       </c>
       <c r="BC92" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD92" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE92" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="93">
@@ -15067,13 +15067,13 @@
         <v>2009</v>
       </c>
       <c r="BC93" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD93" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE93" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="94">
@@ -15224,13 +15224,13 @@
         <v>2009</v>
       </c>
       <c r="BC94" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD94" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE94" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="95">
@@ -15381,13 +15381,13 @@
         <v>2010</v>
       </c>
       <c r="BC95" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD95" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE95" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="96">
@@ -15538,13 +15538,13 @@
         <v>2010</v>
       </c>
       <c r="BC96" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD96" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE96" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="97">
@@ -15695,13 +15695,13 @@
         <v>2010</v>
       </c>
       <c r="BC97" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD97" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE97" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="98">
@@ -15862,13 +15862,13 @@
         <v>2010</v>
       </c>
       <c r="BC98" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD98" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE98" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="99">
@@ -16029,13 +16029,13 @@
         <v>2010</v>
       </c>
       <c r="BC99" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BD99" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE99" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="100">
@@ -16196,13 +16196,13 @@
         <v>2010</v>
       </c>
       <c r="BC100" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD100" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE100" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="101">
@@ -16363,13 +16363,13 @@
         <v>2010</v>
       </c>
       <c r="BC101" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD101" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
       <c r="BE101" t="n">
-        <v>1111.7</v>
+        <v>1009.7</v>
       </c>
     </row>
     <row r="102">
@@ -16530,13 +16530,13 @@
         <v>2010</v>
       </c>
       <c r="BC102" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD102" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE102" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="103">
@@ -16697,13 +16697,13 @@
         <v>2010</v>
       </c>
       <c r="BC103" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD103" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE103" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="104">
@@ -16864,13 +16864,13 @@
         <v>2010</v>
       </c>
       <c r="BC104" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD104" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE104" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="105">
@@ -17031,13 +17031,13 @@
         <v>2010</v>
       </c>
       <c r="BC105" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD105" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE105" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="106">
@@ -17198,13 +17198,13 @@
         <v>2010</v>
       </c>
       <c r="BC106" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD106" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE106" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="107">
@@ -17365,13 +17365,13 @@
         <v>2011</v>
       </c>
       <c r="BC107" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD107" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE107" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="108">
@@ -17532,13 +17532,13 @@
         <v>2011</v>
       </c>
       <c r="BC108" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD108" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE108" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="109">
@@ -17699,13 +17699,13 @@
         <v>2011</v>
       </c>
       <c r="BC109" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD109" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE109" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="110">
@@ -17866,13 +17866,13 @@
         <v>2011</v>
       </c>
       <c r="BC110" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD110" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE110" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="111">
@@ -18033,13 +18033,13 @@
         <v>2011</v>
       </c>
       <c r="BC111" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BD111" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE111" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="112">
@@ -18200,13 +18200,13 @@
         <v>2011</v>
       </c>
       <c r="BC112" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD112" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE112" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="113">
@@ -18367,13 +18367,13 @@
         <v>2011</v>
       </c>
       <c r="BC113" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD113" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
       <c r="BE113" t="n">
-        <v>1236.1</v>
+        <v>1170.3</v>
       </c>
     </row>
     <row r="114">
@@ -18534,13 +18534,13 @@
         <v>2011</v>
       </c>
       <c r="BC114" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD114" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE114" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="115">
@@ -18701,13 +18701,13 @@
         <v>2011</v>
       </c>
       <c r="BC115" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD115" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE115" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="116">
@@ -18868,13 +18868,13 @@
         <v>2011</v>
       </c>
       <c r="BC116" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD116" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE116" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="117">
@@ -19035,13 +19035,13 @@
         <v>2011</v>
       </c>
       <c r="BC117" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD117" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE117" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="118">
@@ -19202,13 +19202,13 @@
         <v>2011</v>
       </c>
       <c r="BC118" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD118" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE118" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="119">
@@ -19369,13 +19369,13 @@
         <v>2012</v>
       </c>
       <c r="BC119" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD119" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE119" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="120">
@@ -19536,13 +19536,13 @@
         <v>2012</v>
       </c>
       <c r="BC120" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD120" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE120" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="121">
@@ -19703,13 +19703,13 @@
         <v>2012</v>
       </c>
       <c r="BC121" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD121" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE121" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="122">
@@ -19870,13 +19870,13 @@
         <v>2012</v>
       </c>
       <c r="BC122" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD122" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE122" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="123">
@@ -20037,13 +20037,13 @@
         <v>2012</v>
       </c>
       <c r="BC123" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BD123" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE123" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="124">
@@ -20204,13 +20204,13 @@
         <v>2012</v>
       </c>
       <c r="BC124" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD124" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE124" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="125">
@@ -20371,13 +20371,13 @@
         <v>2012</v>
       </c>
       <c r="BC125" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD125" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
       <c r="BE125" t="n">
-        <v>1030</v>
+        <v>955.2</v>
       </c>
     </row>
     <row r="126">
@@ -20538,13 +20538,13 @@
         <v>2012</v>
       </c>
       <c r="BC126" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD126" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE126" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="127">
@@ -20705,13 +20705,13 @@
         <v>2012</v>
       </c>
       <c r="BC127" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD127" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE127" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="128">
@@ -20872,13 +20872,13 @@
         <v>2012</v>
       </c>
       <c r="BC128" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD128" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE128" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="129">
@@ -21039,13 +21039,13 @@
         <v>2012</v>
       </c>
       <c r="BC129" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD129" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE129" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="130">
@@ -21206,13 +21206,13 @@
         <v>2012</v>
       </c>
       <c r="BC130" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD130" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE130" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="131">
@@ -21373,13 +21373,13 @@
         <v>2013</v>
       </c>
       <c r="BC131" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD131" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE131" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="132">
@@ -21540,13 +21540,13 @@
         <v>2013</v>
       </c>
       <c r="BC132" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD132" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE132" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="133">
@@ -21707,13 +21707,13 @@
         <v>2013</v>
       </c>
       <c r="BC133" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD133" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE133" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="134">
@@ -21874,13 +21874,13 @@
         <v>2013</v>
       </c>
       <c r="BC134" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD134" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE134" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="135">
@@ -22041,13 +22041,13 @@
         <v>2013</v>
       </c>
       <c r="BC135" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BD135" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE135" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="136">
@@ -22208,13 +22208,13 @@
         <v>2013</v>
       </c>
       <c r="BC136" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD136" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE136" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="137">
@@ -22375,13 +22375,13 @@
         <v>2013</v>
       </c>
       <c r="BC137" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD137" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
       <c r="BE137" t="n">
-        <v>1401.5</v>
+        <v>1087.9</v>
       </c>
     </row>
     <row r="138">
@@ -22542,13 +22542,13 @@
         <v>2013</v>
       </c>
       <c r="BC138" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD138" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE138" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="139">
@@ -22709,13 +22709,13 @@
         <v>2013</v>
       </c>
       <c r="BC139" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD139" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE139" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="140">
@@ -22876,13 +22876,13 @@
         <v>2013</v>
       </c>
       <c r="BC140" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD140" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE140" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="141">
@@ -23043,13 +23043,13 @@
         <v>2013</v>
       </c>
       <c r="BC141" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD141" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE141" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="142">
@@ -23210,13 +23210,13 @@
         <v>2013</v>
       </c>
       <c r="BC142" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD142" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE142" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="143">
@@ -23377,13 +23377,13 @@
         <v>2014</v>
       </c>
       <c r="BC143" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD143" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE143" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="144">
@@ -23544,13 +23544,13 @@
         <v>2014</v>
       </c>
       <c r="BC144" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD144" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE144" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="145">
@@ -23711,13 +23711,13 @@
         <v>2014</v>
       </c>
       <c r="BC145" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD145" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE145" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="146">
@@ -23878,13 +23878,13 @@
         <v>2014</v>
       </c>
       <c r="BC146" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD146" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE146" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="147">
@@ -24045,13 +24045,13 @@
         <v>2014</v>
       </c>
       <c r="BC147" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BD147" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE147" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="148">
@@ -24212,13 +24212,13 @@
         <v>2014</v>
       </c>
       <c r="BC148" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD148" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE148" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="149">
@@ -24379,13 +24379,13 @@
         <v>2014</v>
       </c>
       <c r="BC149" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD149" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
       <c r="BE149" t="n">
-        <v>1391.1</v>
+        <v>1339.6</v>
       </c>
     </row>
     <row r="150">
@@ -24546,13 +24546,13 @@
         <v>2014</v>
       </c>
       <c r="BC150" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD150" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE150" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="151">
@@ -24713,13 +24713,13 @@
         <v>2014</v>
       </c>
       <c r="BC151" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD151" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE151" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="152">
@@ -24880,13 +24880,13 @@
         <v>2014</v>
       </c>
       <c r="BC152" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD152" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE152" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="153">
@@ -25047,13 +25047,13 @@
         <v>2014</v>
       </c>
       <c r="BC153" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD153" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE153" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="154">
@@ -25214,13 +25214,13 @@
         <v>2014</v>
       </c>
       <c r="BC154" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD154" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE154" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="155">
@@ -25381,13 +25381,13 @@
         <v>2015</v>
       </c>
       <c r="BC155" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD155" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE155" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="156">
@@ -25548,13 +25548,13 @@
         <v>2015</v>
       </c>
       <c r="BC156" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD156" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE156" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="157">
@@ -25715,13 +25715,13 @@
         <v>2015</v>
       </c>
       <c r="BC157" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD157" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE157" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="158">
@@ -25882,13 +25882,13 @@
         <v>2015</v>
       </c>
       <c r="BC158" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD158" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE158" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="159">
@@ -26049,13 +26049,13 @@
         <v>2015</v>
       </c>
       <c r="BC159" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BD159" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE159" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="160">
@@ -26216,13 +26216,13 @@
         <v>2015</v>
       </c>
       <c r="BC160" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD160" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE160" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="161">
@@ -26383,13 +26383,13 @@
         <v>2015</v>
       </c>
       <c r="BC161" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD161" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
       <c r="BE161" t="n">
-        <v>1615</v>
+        <v>1571.4</v>
       </c>
     </row>
     <row r="162">
@@ -26550,13 +26550,13 @@
         <v>2015</v>
       </c>
       <c r="BC162" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD162" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE162" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="163">
@@ -26717,13 +26717,13 @@
         <v>2015</v>
       </c>
       <c r="BC163" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD163" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE163" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="164">
@@ -26884,13 +26884,13 @@
         <v>2015</v>
       </c>
       <c r="BC164" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD164" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE164" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="165">
@@ -27051,13 +27051,13 @@
         <v>2015</v>
       </c>
       <c r="BC165" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD165" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE165" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="166">
@@ -27218,13 +27218,13 @@
         <v>2015</v>
       </c>
       <c r="BC166" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD166" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE166" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="167">
@@ -27385,13 +27385,13 @@
         <v>2016</v>
       </c>
       <c r="BC167" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD167" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE167" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="168">
@@ -27552,13 +27552,13 @@
         <v>2016</v>
       </c>
       <c r="BC168" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD168" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE168" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="169">
@@ -27721,13 +27721,13 @@
         <v>2016</v>
       </c>
       <c r="BC169" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD169" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE169" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="170">
@@ -27890,13 +27890,13 @@
         <v>2016</v>
       </c>
       <c r="BC170" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD170" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE170" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="171">
@@ -28059,13 +28059,13 @@
         <v>2016</v>
       </c>
       <c r="BC171" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BD171" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE171" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="172">
@@ -28228,13 +28228,13 @@
         <v>2016</v>
       </c>
       <c r="BC172" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD172" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE172" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="173">
@@ -28397,13 +28397,13 @@
         <v>2016</v>
       </c>
       <c r="BC173" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD173" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
       <c r="BE173" t="n">
-        <v>618.2</v>
+        <v>598.6</v>
       </c>
     </row>
     <row r="174">
@@ -28566,13 +28566,13 @@
         <v>2016</v>
       </c>
       <c r="BC174" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD174" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE174" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="175">
@@ -28735,13 +28735,13 @@
         <v>2016</v>
       </c>
       <c r="BC175" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD175" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE175" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="176">
@@ -28904,13 +28904,13 @@
         <v>2016</v>
       </c>
       <c r="BC176" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD176" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE176" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="177">
@@ -29073,13 +29073,13 @@
         <v>2016</v>
       </c>
       <c r="BC177" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD177" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE177" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="178">
@@ -29242,13 +29242,13 @@
         <v>2016</v>
       </c>
       <c r="BC178" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD178" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE178" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="179">
@@ -29411,13 +29411,13 @@
         <v>2017</v>
       </c>
       <c r="BC179" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD179" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE179" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="180">
@@ -29580,13 +29580,13 @@
         <v>2017</v>
       </c>
       <c r="BC180" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD180" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE180" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="181">
@@ -29749,13 +29749,13 @@
         <v>2017</v>
       </c>
       <c r="BC181" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD181" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE181" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="182">
@@ -29918,13 +29918,13 @@
         <v>2017</v>
       </c>
       <c r="BC182" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD182" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE182" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="183">
@@ -30087,13 +30087,13 @@
         <v>2017</v>
       </c>
       <c r="BC183" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BD183" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE183" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="184">
@@ -30256,13 +30256,13 @@
         <v>2017</v>
       </c>
       <c r="BC184" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD184" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE184" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="185">
@@ -30425,13 +30425,13 @@
         <v>2017</v>
       </c>
       <c r="BC185" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD185" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
       <c r="BE185" t="n">
-        <v>1780.2</v>
+        <v>1553.1</v>
       </c>
     </row>
     <row r="186">
@@ -30594,13 +30594,13 @@
         <v>2017</v>
       </c>
       <c r="BC186" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD186" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE186" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="187">
@@ -30763,13 +30763,13 @@
         <v>2017</v>
       </c>
       <c r="BC187" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD187" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE187" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="188">
@@ -30932,13 +30932,13 @@
         <v>2017</v>
       </c>
       <c r="BC188" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD188" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE188" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="189">
@@ -31101,13 +31101,13 @@
         <v>2017</v>
       </c>
       <c r="BC189" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD189" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE189" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="190">
@@ -31270,13 +31270,13 @@
         <v>2017</v>
       </c>
       <c r="BC190" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD190" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE190" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="191">
@@ -31439,13 +31439,13 @@
         <v>2018</v>
       </c>
       <c r="BC191" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD191" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE191" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="192">
@@ -31608,13 +31608,13 @@
         <v>2018</v>
       </c>
       <c r="BC192" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD192" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE192" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="193">
@@ -31777,13 +31777,13 @@
         <v>2018</v>
       </c>
       <c r="BC193" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD193" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE193" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="194">
@@ -31950,13 +31950,13 @@
         <v>2018</v>
       </c>
       <c r="BC194" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD194" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE194" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="195">
@@ -32123,13 +32123,13 @@
         <v>2018</v>
       </c>
       <c r="BC195" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BD195" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE195" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="196">
@@ -32296,13 +32296,13 @@
         <v>2018</v>
       </c>
       <c r="BC196" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD196" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE196" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="197">
@@ -32469,13 +32469,13 @@
         <v>2018</v>
       </c>
       <c r="BC197" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD197" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
       <c r="BE197" t="n">
-        <v>842.3000000000001</v>
+        <v>813.7</v>
       </c>
     </row>
     <row r="198">
@@ -32642,13 +32642,13 @@
         <v>2018</v>
       </c>
       <c r="BC198" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD198" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE198" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="199">
@@ -32815,13 +32815,13 @@
         <v>2018</v>
       </c>
       <c r="BC199" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD199" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE199" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="200">
@@ -32988,13 +32988,13 @@
         <v>2018</v>
       </c>
       <c r="BC200" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD200" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE200" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="201">
@@ -33161,13 +33161,13 @@
         <v>2018</v>
       </c>
       <c r="BC201" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD201" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE201" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="202">
@@ -33334,13 +33334,13 @@
         <v>2018</v>
       </c>
       <c r="BC202" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD202" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE202" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="203">
@@ -33507,13 +33507,13 @@
         <v>2019</v>
       </c>
       <c r="BC203" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD203" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE203" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="204">
@@ -33680,13 +33680,13 @@
         <v>2019</v>
       </c>
       <c r="BC204" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD204" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE204" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="205">
@@ -33853,13 +33853,13 @@
         <v>2019</v>
       </c>
       <c r="BC205" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD205" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE205" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="206">
@@ -34026,13 +34026,13 @@
         <v>2019</v>
       </c>
       <c r="BC206" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD206" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE206" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="207">
@@ -34199,13 +34199,13 @@
         <v>2019</v>
       </c>
       <c r="BC207" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BD207" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE207" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="208">
@@ -34372,13 +34372,13 @@
         <v>2019</v>
       </c>
       <c r="BC208" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD208" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE208" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="209">
@@ -34545,13 +34545,13 @@
         <v>2019</v>
       </c>
       <c r="BC209" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD209" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
       <c r="BE209" t="n">
-        <v>1403.3</v>
+        <v>1368.3</v>
       </c>
     </row>
     <row r="210">
@@ -34718,13 +34718,13 @@
         <v>2019</v>
       </c>
       <c r="BC210" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD210" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE210" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="211">
@@ -34891,13 +34891,13 @@
         <v>2019</v>
       </c>
       <c r="BC211" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD211" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE211" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="212">
@@ -35064,13 +35064,13 @@
         <v>2019</v>
       </c>
       <c r="BC212" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD212" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE212" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="213">
@@ -35237,13 +35237,13 @@
         <v>2019</v>
       </c>
       <c r="BC213" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD213" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE213" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="214">
@@ -35410,13 +35410,13 @@
         <v>2019</v>
       </c>
       <c r="BC214" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD214" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE214" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="215">
@@ -35583,13 +35583,13 @@
         <v>2020</v>
       </c>
       <c r="BC215" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD215" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE215" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="216">
@@ -35756,13 +35756,13 @@
         <v>2020</v>
       </c>
       <c r="BC216" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD216" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE216" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="217">
@@ -35929,13 +35929,13 @@
         <v>2020</v>
       </c>
       <c r="BC217" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD217" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE217" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="218">
@@ -36102,13 +36102,13 @@
         <v>2020</v>
       </c>
       <c r="BC218" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD218" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE218" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="219">
@@ -36275,13 +36275,13 @@
         <v>2020</v>
       </c>
       <c r="BC219" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BD219" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE219" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="220">
@@ -36448,13 +36448,13 @@
         <v>2020</v>
       </c>
       <c r="BC220" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD220" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE220" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="221">
@@ -36621,13 +36621,13 @@
         <v>2020</v>
       </c>
       <c r="BC221" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD221" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
       <c r="BE221" t="n">
-        <v>1290.6</v>
+        <v>1243.5</v>
       </c>
     </row>
     <row r="222">
@@ -36794,13 +36794,13 @@
         <v>2020</v>
       </c>
       <c r="BC222" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD222" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE222" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="223">
@@ -36967,13 +36967,13 @@
         <v>2020</v>
       </c>
       <c r="BC223" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD223" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE223" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="224">
@@ -37140,13 +37140,13 @@
         <v>2020</v>
       </c>
       <c r="BC224" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD224" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE224" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="225">
@@ -37313,13 +37313,13 @@
         <v>2020</v>
       </c>
       <c r="BC225" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD225" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE225" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="226">
@@ -37486,13 +37486,13 @@
         <v>2020</v>
       </c>
       <c r="BC226" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD226" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE226" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="227">
@@ -37659,13 +37659,13 @@
         <v>2021</v>
       </c>
       <c r="BC227" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD227" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE227" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="228">
@@ -37832,13 +37832,13 @@
         <v>2021</v>
       </c>
       <c r="BC228" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD228" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE228" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="229">
@@ -38005,13 +38005,13 @@
         <v>2021</v>
       </c>
       <c r="BC229" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD229" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE229" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="230">
@@ -38178,13 +38178,13 @@
         <v>2021</v>
       </c>
       <c r="BC230" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD230" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE230" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="231">
@@ -38351,13 +38351,13 @@
         <v>2021</v>
       </c>
       <c r="BC231" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BD231" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE231" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="232">
@@ -38524,13 +38524,13 @@
         <v>2021</v>
       </c>
       <c r="BC232" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD232" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE232" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="233">
@@ -38697,13 +38697,13 @@
         <v>2021</v>
       </c>
       <c r="BC233" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD233" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
       <c r="BE233" t="n">
-        <v>1262.2</v>
+        <v>1220.9</v>
       </c>
     </row>
     <row r="234">
@@ -38870,13 +38870,13 @@
         <v>2021</v>
       </c>
       <c r="BC234" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD234" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE234" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="235">
@@ -39043,13 +39043,13 @@
         <v>2021</v>
       </c>
       <c r="BC235" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD235" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE235" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="236">
@@ -39216,13 +39216,13 @@
         <v>2021</v>
       </c>
       <c r="BC236" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD236" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE236" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="237">
@@ -39389,13 +39389,13 @@
         <v>2021</v>
       </c>
       <c r="BC237" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD237" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE237" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="238">
@@ -39562,13 +39562,13 @@
         <v>2021</v>
       </c>
       <c r="BC238" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD238" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE238" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="239">
@@ -39735,13 +39735,13 @@
         <v>2022</v>
       </c>
       <c r="BC239" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD239" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE239" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="240">
@@ -39908,13 +39908,13 @@
         <v>2022</v>
       </c>
       <c r="BC240" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD240" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE240" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="241">
@@ -40081,13 +40081,13 @@
         <v>2022</v>
       </c>
       <c r="BC241" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD241" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE241" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="242">
@@ -40254,13 +40254,13 @@
         <v>2022</v>
       </c>
       <c r="BC242" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD242" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE242" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="243">
@@ -40427,13 +40427,13 @@
         <v>2022</v>
       </c>
       <c r="BC243" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BD243" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE243" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="244">
@@ -40600,13 +40600,13 @@
         <v>2022</v>
       </c>
       <c r="BC244" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD244" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE244" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="245">
@@ -40773,13 +40773,13 @@
         <v>2022</v>
       </c>
       <c r="BC245" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD245" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
       <c r="BE245" t="n">
-        <v>1793.5</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="246">
@@ -40946,13 +40946,13 @@
         <v>2022</v>
       </c>
       <c r="BC246" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD246" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE246" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="247">
@@ -41119,13 +41119,13 @@
         <v>2022</v>
       </c>
       <c r="BC247" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD247" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE247" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="248">
@@ -41292,13 +41292,13 @@
         <v>2022</v>
       </c>
       <c r="BC248" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD248" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE248" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="249">
@@ -41465,13 +41465,13 @@
         <v>2022</v>
       </c>
       <c r="BC249" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD249" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE249" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="250">
@@ -41638,13 +41638,13 @@
         <v>2022</v>
       </c>
       <c r="BC250" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD250" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE250" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="251">
@@ -41811,13 +41811,13 @@
         <v>2023</v>
       </c>
       <c r="BC251" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD251" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE251" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="252">
@@ -41984,13 +41984,13 @@
         <v>2023</v>
       </c>
       <c r="BC252" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD252" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE252" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="253">
@@ -42157,13 +42157,13 @@
         <v>2023</v>
       </c>
       <c r="BC253" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD253" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE253" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="254">
@@ -42330,13 +42330,13 @@
         <v>2023</v>
       </c>
       <c r="BC254" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD254" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE254" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="255">
@@ -42461,13 +42461,13 @@
         <v>2023</v>
       </c>
       <c r="BC255" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BD255" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE255" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="256">
@@ -42592,13 +42592,13 @@
         <v>2023</v>
       </c>
       <c r="BC256" t="n">
-        <v>663.4</v>
+        <v>653.4</v>
       </c>
       <c r="BD256" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE256" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="257">
@@ -42724,10 +42724,10 @@
       </c>
       <c r="BC257" t="inlineStr"/>
       <c r="BD257" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
       <c r="BE257" t="n">
-        <v>1125.7</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="258">
@@ -42853,10 +42853,10 @@
       </c>
       <c r="BC258" t="inlineStr"/>
       <c r="BD258" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BE258" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
     </row>
     <row r="259">
@@ -42982,10 +42982,10 @@
       </c>
       <c r="BC259" t="inlineStr"/>
       <c r="BD259" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BE259" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
     </row>
     <row r="260">
@@ -43099,10 +43099,10 @@
       </c>
       <c r="BC260" t="inlineStr"/>
       <c r="BD260" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BE260" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
     </row>
     <row r="261">
@@ -43208,10 +43208,10 @@
       </c>
       <c r="BC261" t="inlineStr"/>
       <c r="BD261" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BE261" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
     </row>
     <row r="262">
@@ -43305,10 +43305,10 @@
       </c>
       <c r="BC262" t="inlineStr"/>
       <c r="BD262" t="n">
-        <v>1493</v>
+        <v>1462.2</v>
       </c>
       <c r="BE262" t="n">
-        <v>1389.1</v>
+        <v>1336.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Meteo Var stats added
</commit_message>
<xml_diff>
--- a/Output/Excel/df_month.xlsx
+++ b/Output/Excel/df_month.xlsx
@@ -16864,9 +16864,7 @@
       <c r="BH98" t="n">
         <v>1009.7</v>
       </c>
-      <c r="BI98" t="n">
-        <v>1260.316486298508</v>
-      </c>
+      <c r="BI98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
@@ -17043,9 +17041,7 @@
       <c r="BH99" t="n">
         <v>1009.7</v>
       </c>
-      <c r="BI99" t="n">
-        <v>1260.316486298508</v>
-      </c>
+      <c r="BI99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
@@ -17222,9 +17218,7 @@
       <c r="BH100" t="n">
         <v>1170.3</v>
       </c>
-      <c r="BI100" t="n">
-        <v>1260.316486298508</v>
-      </c>
+      <c r="BI100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
@@ -17401,9 +17395,7 @@
       <c r="BH101" t="n">
         <v>1170.3</v>
       </c>
-      <c r="BI101" t="n">
-        <v>1260.316486298508</v>
-      </c>
+      <c r="BI101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
@@ -17580,9 +17572,7 @@
       <c r="BH102" t="n">
         <v>1170.3</v>
       </c>
-      <c r="BI102" t="n">
-        <v>1260.316486298508</v>
-      </c>
+      <c r="BI102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
@@ -17759,9 +17749,7 @@
       <c r="BH103" t="n">
         <v>1170.3</v>
       </c>
-      <c r="BI103" t="n">
-        <v>1260.316486298508</v>
-      </c>
+      <c r="BI103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
@@ -17930,7 +17918,7 @@
         <v>40360</v>
       </c>
       <c r="BF104" t="n">
-        <v>1260.316486298508</v>
+        <v>1087.9</v>
       </c>
       <c r="BG104" t="n">
         <v>955.2</v>
@@ -19013,7 +19001,7 @@
         <v>1170.3</v>
       </c>
       <c r="BI110" t="n">
-        <v>1306.994874679935</v>
+        <v>1260.316486298508</v>
       </c>
     </row>
     <row r="111">
@@ -19192,7 +19180,7 @@
         <v>1170.3</v>
       </c>
       <c r="BI111" t="n">
-        <v>1306.994874679935</v>
+        <v>1260.316486298508</v>
       </c>
     </row>
     <row r="112">
@@ -19371,7 +19359,7 @@
         <v>955.2</v>
       </c>
       <c r="BI112" t="n">
-        <v>1306.994874679935</v>
+        <v>1260.316486298508</v>
       </c>
     </row>
     <row r="113">
@@ -19550,7 +19538,7 @@
         <v>955.2</v>
       </c>
       <c r="BI113" t="n">
-        <v>1306.994874679935</v>
+        <v>1260.316486298508</v>
       </c>
     </row>
     <row r="114">
@@ -19729,7 +19717,7 @@
         <v>955.2</v>
       </c>
       <c r="BI114" t="n">
-        <v>1306.994874679935</v>
+        <v>1260.316486298508</v>
       </c>
     </row>
     <row r="115">
@@ -19908,7 +19896,7 @@
         <v>955.2</v>
       </c>
       <c r="BI115" t="n">
-        <v>1306.994874679935</v>
+        <v>1260.316486298508</v>
       </c>
     </row>
     <row r="116">
@@ -20078,7 +20066,7 @@
         <v>40725</v>
       </c>
       <c r="BF116" t="n">
-        <v>1306.994874679935</v>
+        <v>1339.6</v>
       </c>
       <c r="BG116" t="n">
         <v>1087.9</v>
@@ -21161,7 +21149,7 @@
         <v>955.2</v>
       </c>
       <c r="BI122" t="n">
-        <v>583.479854767828</v>
+        <v>1306.994874679935</v>
       </c>
     </row>
     <row r="123">
@@ -21340,7 +21328,7 @@
         <v>955.2</v>
       </c>
       <c r="BI123" t="n">
-        <v>583.479854767828</v>
+        <v>1306.994874679935</v>
       </c>
     </row>
     <row r="124">
@@ -21519,7 +21507,7 @@
         <v>1087.9</v>
       </c>
       <c r="BI124" t="n">
-        <v>583.479854767828</v>
+        <v>1306.994874679935</v>
       </c>
     </row>
     <row r="125">
@@ -21698,7 +21686,7 @@
         <v>1087.9</v>
       </c>
       <c r="BI125" t="n">
-        <v>583.479854767828</v>
+        <v>1306.994874679935</v>
       </c>
     </row>
     <row r="126">
@@ -21877,7 +21865,7 @@
         <v>1087.9</v>
       </c>
       <c r="BI126" t="n">
-        <v>583.479854767828</v>
+        <v>1306.994874679935</v>
       </c>
     </row>
     <row r="127">
@@ -22056,7 +22044,7 @@
         <v>1087.9</v>
       </c>
       <c r="BI127" t="n">
-        <v>583.479854767828</v>
+        <v>1306.994874679935</v>
       </c>
     </row>
     <row r="128">
@@ -22226,7 +22214,7 @@
         <v>41091</v>
       </c>
       <c r="BF128" t="n">
-        <v>583.479854767828</v>
+        <v>1571.4</v>
       </c>
       <c r="BG128" t="n">
         <v>1339.6</v>
@@ -23309,7 +23297,7 @@
         <v>1087.9</v>
       </c>
       <c r="BI134" t="n">
-        <v>1503.977673649553</v>
+        <v>583.479854767828</v>
       </c>
     </row>
     <row r="135">
@@ -23488,7 +23476,7 @@
         <v>1087.9</v>
       </c>
       <c r="BI135" t="n">
-        <v>1503.977673649553</v>
+        <v>583.479854767828</v>
       </c>
     </row>
     <row r="136">
@@ -23667,7 +23655,7 @@
         <v>1339.6</v>
       </c>
       <c r="BI136" t="n">
-        <v>1503.977673649553</v>
+        <v>583.479854767828</v>
       </c>
     </row>
     <row r="137">
@@ -23846,7 +23834,7 @@
         <v>1339.6</v>
       </c>
       <c r="BI137" t="n">
-        <v>1503.977673649553</v>
+        <v>583.479854767828</v>
       </c>
     </row>
     <row r="138">
@@ -24025,7 +24013,7 @@
         <v>1339.6</v>
       </c>
       <c r="BI138" t="n">
-        <v>1503.977673649553</v>
+        <v>583.479854767828</v>
       </c>
     </row>
     <row r="139">
@@ -24204,7 +24192,7 @@
         <v>1339.6</v>
       </c>
       <c r="BI139" t="n">
-        <v>1503.977673649553</v>
+        <v>583.479854767828</v>
       </c>
     </row>
     <row r="140">
@@ -24374,7 +24362,7 @@
         <v>41456</v>
       </c>
       <c r="BF140" t="n">
-        <v>1503.977673649553</v>
+        <v>598.6</v>
       </c>
       <c r="BG140" t="n">
         <v>1571.4</v>
@@ -25457,7 +25445,7 @@
         <v>1339.6</v>
       </c>
       <c r="BI146" t="n">
-        <v>731.9171298207634</v>
+        <v>1503.977673649553</v>
       </c>
     </row>
     <row r="147">
@@ -25636,7 +25624,7 @@
         <v>1339.6</v>
       </c>
       <c r="BI147" t="n">
-        <v>731.9171298207634</v>
+        <v>1503.977673649553</v>
       </c>
     </row>
     <row r="148">
@@ -25815,7 +25803,7 @@
         <v>1571.4</v>
       </c>
       <c r="BI148" t="n">
-        <v>731.9171298207634</v>
+        <v>1503.977673649553</v>
       </c>
     </row>
     <row r="149">
@@ -25994,7 +25982,7 @@
         <v>1571.4</v>
       </c>
       <c r="BI149" t="n">
-        <v>731.9171298207634</v>
+        <v>1503.977673649553</v>
       </c>
     </row>
     <row r="150">
@@ -26173,7 +26161,7 @@
         <v>1571.4</v>
       </c>
       <c r="BI150" t="n">
-        <v>731.9171298207634</v>
+        <v>1503.977673649553</v>
       </c>
     </row>
     <row r="151">
@@ -26352,7 +26340,7 @@
         <v>1571.4</v>
       </c>
       <c r="BI151" t="n">
-        <v>731.9171298207634</v>
+        <v>1503.977673649553</v>
       </c>
     </row>
     <row r="152">
@@ -26522,7 +26510,7 @@
         <v>41821</v>
       </c>
       <c r="BF152" t="n">
-        <v>731.9171298207634</v>
+        <v>1553.1</v>
       </c>
       <c r="BG152" t="n">
         <v>598.6</v>
@@ -27605,7 +27593,7 @@
         <v>1571.4</v>
       </c>
       <c r="BI158" t="n">
-        <v>1120.28132115423</v>
+        <v>731.9171298207634</v>
       </c>
     </row>
     <row r="159">
@@ -27784,7 +27772,7 @@
         <v>1571.4</v>
       </c>
       <c r="BI159" t="n">
-        <v>1120.28132115423</v>
+        <v>731.9171298207634</v>
       </c>
     </row>
     <row r="160">
@@ -27963,7 +27951,7 @@
         <v>598.6</v>
       </c>
       <c r="BI160" t="n">
-        <v>1120.28132115423</v>
+        <v>731.9171298207634</v>
       </c>
     </row>
     <row r="161">
@@ -28142,7 +28130,7 @@
         <v>598.6</v>
       </c>
       <c r="BI161" t="n">
-        <v>1120.28132115423</v>
+        <v>731.9171298207634</v>
       </c>
     </row>
     <row r="162">
@@ -28321,7 +28309,7 @@
         <v>598.6</v>
       </c>
       <c r="BI162" t="n">
-        <v>1120.28132115423</v>
+        <v>731.9171298207634</v>
       </c>
     </row>
     <row r="163">
@@ -28500,7 +28488,7 @@
         <v>598.6</v>
       </c>
       <c r="BI163" t="n">
-        <v>1120.28132115423</v>
+        <v>731.9171298207634</v>
       </c>
     </row>
     <row r="164">
@@ -28670,7 +28658,7 @@
         <v>42186</v>
       </c>
       <c r="BF164" t="n">
-        <v>1120.28132115423</v>
+        <v>813.7</v>
       </c>
       <c r="BG164" t="n">
         <v>1553.1</v>
@@ -29757,7 +29745,7 @@
         <v>598.6</v>
       </c>
       <c r="BI170" t="n">
-        <v>1288.323519327364</v>
+        <v>1120.28132115423</v>
       </c>
     </row>
     <row r="171">
@@ -29938,7 +29926,7 @@
         <v>598.6</v>
       </c>
       <c r="BI171" t="n">
-        <v>1288.323519327364</v>
+        <v>1120.28132115423</v>
       </c>
     </row>
     <row r="172">
@@ -30119,7 +30107,7 @@
         <v>1553.1</v>
       </c>
       <c r="BI172" t="n">
-        <v>1288.323519327364</v>
+        <v>1120.28132115423</v>
       </c>
     </row>
     <row r="173">
@@ -30300,7 +30288,7 @@
         <v>1553.1</v>
       </c>
       <c r="BI173" t="n">
-        <v>1288.323519327364</v>
+        <v>1120.28132115423</v>
       </c>
     </row>
     <row r="174">
@@ -30481,7 +30469,7 @@
         <v>1553.1</v>
       </c>
       <c r="BI174" t="n">
-        <v>1288.323519327364</v>
+        <v>1120.28132115423</v>
       </c>
     </row>
     <row r="175">
@@ -30662,7 +30650,7 @@
         <v>1553.1</v>
       </c>
       <c r="BI175" t="n">
-        <v>1288.323519327364</v>
+        <v>1120.28132115423</v>
       </c>
     </row>
     <row r="176">
@@ -30834,7 +30822,7 @@
         <v>42552</v>
       </c>
       <c r="BF176" t="n">
-        <v>1288.323519327364</v>
+        <v>1368.3</v>
       </c>
       <c r="BG176" t="n">
         <v>813.7</v>
@@ -31929,7 +31917,7 @@
         <v>1553.1</v>
       </c>
       <c r="BI182" t="n">
-        <v>1055.865145187862</v>
+        <v>1288.323519327364</v>
       </c>
     </row>
     <row r="183">
@@ -32110,7 +32098,7 @@
         <v>1553.1</v>
       </c>
       <c r="BI183" t="n">
-        <v>1055.865145187862</v>
+        <v>1288.323519327364</v>
       </c>
     </row>
     <row r="184">
@@ -32291,7 +32279,7 @@
         <v>813.7</v>
       </c>
       <c r="BI184" t="n">
-        <v>1055.865145187862</v>
+        <v>1288.323519327364</v>
       </c>
     </row>
     <row r="185">
@@ -32472,7 +32460,7 @@
         <v>813.7</v>
       </c>
       <c r="BI185" t="n">
-        <v>1055.865145187862</v>
+        <v>1288.323519327364</v>
       </c>
     </row>
     <row r="186">
@@ -32653,7 +32641,7 @@
         <v>813.7</v>
       </c>
       <c r="BI186" t="n">
-        <v>1055.865145187862</v>
+        <v>1288.323519327364</v>
       </c>
     </row>
     <row r="187">
@@ -32834,7 +32822,7 @@
         <v>813.7</v>
       </c>
       <c r="BI187" t="n">
-        <v>1055.865145187862</v>
+        <v>1288.323519327364</v>
       </c>
     </row>
     <row r="188">
@@ -33006,7 +32994,7 @@
         <v>42917</v>
       </c>
       <c r="BF188" t="n">
-        <v>1055.865145187862</v>
+        <v>1243.5</v>
       </c>
       <c r="BG188" t="n">
         <v>1368.3</v>
@@ -34105,7 +34093,7 @@
         <v>813.7</v>
       </c>
       <c r="BI194" t="n">
-        <v>1447.030039824213</v>
+        <v>1055.865145187862</v>
       </c>
     </row>
     <row r="195">
@@ -34290,7 +34278,7 @@
         <v>813.7</v>
       </c>
       <c r="BI195" t="n">
-        <v>1447.030039824213</v>
+        <v>1055.865145187862</v>
       </c>
     </row>
     <row r="196">
@@ -34475,7 +34463,7 @@
         <v>1368.3</v>
       </c>
       <c r="BI196" t="n">
-        <v>1447.030039824213</v>
+        <v>1055.865145187862</v>
       </c>
     </row>
     <row r="197">
@@ -34660,7 +34648,7 @@
         <v>1368.3</v>
       </c>
       <c r="BI197" t="n">
-        <v>1447.030039824213</v>
+        <v>1055.865145187862</v>
       </c>
     </row>
     <row r="198">
@@ -34845,7 +34833,7 @@
         <v>1368.3</v>
       </c>
       <c r="BI198" t="n">
-        <v>1447.030039824213</v>
+        <v>1055.865145187862</v>
       </c>
     </row>
     <row r="199">
@@ -35030,7 +35018,7 @@
         <v>1368.3</v>
       </c>
       <c r="BI199" t="n">
-        <v>1447.030039824213</v>
+        <v>1055.865145187862</v>
       </c>
     </row>
     <row r="200">
@@ -35206,7 +35194,7 @@
         <v>43282</v>
       </c>
       <c r="BF200" t="n">
-        <v>1447.030039824213</v>
+        <v>1220.9</v>
       </c>
       <c r="BG200" t="n">
         <v>1243.5</v>
@@ -36325,7 +36313,7 @@
         <v>1368.3</v>
       </c>
       <c r="BI206" t="n">
-        <v>1166.959709535656</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="207">
@@ -36510,7 +36498,7 @@
         <v>1368.3</v>
       </c>
       <c r="BI207" t="n">
-        <v>1166.959709535656</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="208">
@@ -36695,7 +36683,7 @@
         <v>1243.5</v>
       </c>
       <c r="BI208" t="n">
-        <v>1166.959709535656</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="209">
@@ -36880,7 +36868,7 @@
         <v>1243.5</v>
       </c>
       <c r="BI209" t="n">
-        <v>1166.959709535656</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="210">
@@ -37065,7 +37053,7 @@
         <v>1243.5</v>
       </c>
       <c r="BI210" t="n">
-        <v>1166.959709535656</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="211">
@@ -37250,7 +37238,7 @@
         <v>1243.5</v>
       </c>
       <c r="BI211" t="n">
-        <v>1166.959709535656</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="212">
@@ -37426,7 +37414,7 @@
         <v>43647</v>
       </c>
       <c r="BF212" t="n">
-        <v>1166.959709535656</v>
+        <v>1705</v>
       </c>
       <c r="BG212" t="n">
         <v>1220.9</v>
@@ -38545,7 +38533,7 @@
         <v>1243.5</v>
       </c>
       <c r="BI218" t="n">
-        <v>1447.030039824213</v>
+        <v>1166.959709535656</v>
       </c>
     </row>
     <row r="219">
@@ -38730,7 +38718,7 @@
         <v>1243.5</v>
       </c>
       <c r="BI219" t="n">
-        <v>1447.030039824213</v>
+        <v>1166.959709535656</v>
       </c>
     </row>
     <row r="220">
@@ -38915,7 +38903,7 @@
         <v>1220.9</v>
       </c>
       <c r="BI220" t="n">
-        <v>1447.030039824213</v>
+        <v>1166.959709535656</v>
       </c>
     </row>
     <row r="221">
@@ -39100,7 +39088,7 @@
         <v>1220.9</v>
       </c>
       <c r="BI221" t="n">
-        <v>1447.030039824213</v>
+        <v>1166.959709535656</v>
       </c>
     </row>
     <row r="222">
@@ -39285,7 +39273,7 @@
         <v>1220.9</v>
       </c>
       <c r="BI222" t="n">
-        <v>1447.030039824213</v>
+        <v>1166.959709535656</v>
       </c>
     </row>
     <row r="223">
@@ -39470,7 +39458,7 @@
         <v>1220.9</v>
       </c>
       <c r="BI223" t="n">
-        <v>1447.030039824213</v>
+        <v>1166.959709535656</v>
       </c>
     </row>
     <row r="224">
@@ -39646,7 +39634,7 @@
         <v>44013</v>
       </c>
       <c r="BF224" t="n">
-        <v>1447.030039824213</v>
+        <v>1105</v>
       </c>
       <c r="BG224" t="n">
         <v>1705</v>
@@ -40765,7 +40753,7 @@
         <v>1220.9</v>
       </c>
       <c r="BI230" t="n">
-        <v>1213.638097917082</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="231">
@@ -40950,7 +40938,7 @@
         <v>1220.9</v>
       </c>
       <c r="BI231" t="n">
-        <v>1213.638097917082</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="232">
@@ -41135,7 +41123,7 @@
         <v>1705</v>
       </c>
       <c r="BI232" t="n">
-        <v>1213.638097917082</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="233">
@@ -41320,7 +41308,7 @@
         <v>1705</v>
       </c>
       <c r="BI233" t="n">
-        <v>1213.638097917082</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="234">
@@ -41505,7 +41493,7 @@
         <v>1705</v>
       </c>
       <c r="BI234" t="n">
-        <v>1213.638097917082</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="235">
@@ -41690,7 +41678,7 @@
         <v>1705</v>
       </c>
       <c r="BI235" t="n">
-        <v>1213.638097917082</v>
+        <v>1447.030039824213</v>
       </c>
     </row>
     <row r="236">
@@ -41866,7 +41854,7 @@
         <v>44378</v>
       </c>
       <c r="BF236" t="n">
-        <v>1213.638097917082</v>
+        <v>1336.9</v>
       </c>
       <c r="BG236" t="n">
         <v>1105</v>
@@ -42985,7 +42973,7 @@
         <v>1705</v>
       </c>
       <c r="BI242" t="n">
-        <v>728.1828587502494</v>
+        <v>1213.638097917082</v>
       </c>
     </row>
     <row r="243">
@@ -43170,7 +43158,7 @@
         <v>1705</v>
       </c>
       <c r="BI243" t="n">
-        <v>728.1828587502494</v>
+        <v>1213.638097917082</v>
       </c>
     </row>
     <row r="244">
@@ -43355,7 +43343,7 @@
         <v>1105</v>
       </c>
       <c r="BI244" t="n">
-        <v>728.1828587502494</v>
+        <v>1213.638097917082</v>
       </c>
     </row>
     <row r="245">
@@ -43540,7 +43528,7 @@
         <v>1105</v>
       </c>
       <c r="BI245" t="n">
-        <v>728.1828587502494</v>
+        <v>1213.638097917082</v>
       </c>
     </row>
     <row r="246">
@@ -43725,7 +43713,7 @@
         <v>1105</v>
       </c>
       <c r="BI246" t="n">
-        <v>728.1828587502494</v>
+        <v>1213.638097917082</v>
       </c>
     </row>
     <row r="247">
@@ -43910,7 +43898,7 @@
         <v>1105</v>
       </c>
       <c r="BI247" t="n">
-        <v>728.1828587502494</v>
+        <v>1213.638097917082</v>
       </c>
     </row>
     <row r="248">
@@ -44086,7 +44074,7 @@
         <v>44743</v>
       </c>
       <c r="BF248" t="n">
-        <v>728.1828587502494</v>
+        <v>1462.2</v>
       </c>
       <c r="BG248" t="n">
         <v>1336.9</v>
@@ -45205,7 +45193,7 @@
         <v>1105</v>
       </c>
       <c r="BI254" t="n">
-        <v>714.1793422358214</v>
+        <v>728.1828587502494</v>
       </c>
     </row>
     <row r="255">
@@ -45348,7 +45336,7 @@
         <v>1105</v>
       </c>
       <c r="BI255" t="n">
-        <v>714.1793422358214</v>
+        <v>728.1828587502494</v>
       </c>
     </row>
     <row r="256">
@@ -45491,7 +45479,7 @@
         <v>1336.9</v>
       </c>
       <c r="BI256" t="n">
-        <v>714.1793422358214</v>
+        <v>728.1828587502494</v>
       </c>
     </row>
     <row r="257">
@@ -45632,7 +45620,7 @@
         <v>1336.9</v>
       </c>
       <c r="BI257" t="n">
-        <v>714.1793422358214</v>
+        <v>728.1828587502494</v>
       </c>
     </row>
     <row r="258">
@@ -45773,7 +45761,7 @@
         <v>1336.9</v>
       </c>
       <c r="BI258" t="n">
-        <v>714.1793422358214</v>
+        <v>728.1828587502494</v>
       </c>
     </row>
     <row r="259">
@@ -45914,7 +45902,7 @@
         <v>1336.9</v>
       </c>
       <c r="BI259" t="n">
-        <v>714.1793422358214</v>
+        <v>728.1828587502494</v>
       </c>
     </row>
     <row r="260">
@@ -46034,7 +46022,7 @@
         <v>45108</v>
       </c>
       <c r="BF260" t="n">
-        <v>714.1793422358214</v>
+        <v>653.4</v>
       </c>
       <c r="BG260" t="n">
         <v>1462.2</v>

</xml_diff>